<commit_message>
programa rodando 100% como o original
</commit_message>
<xml_diff>
--- a/pesos/acao.xlsx
+++ b/pesos/acao.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0ba5887f9c16091d/Área de Trabalho/asset alocation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\hub-do-investidor\pesos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="175" documentId="8_{216E35A9-7F35-45D2-BBCC-78FB5489D549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17339873-9CFC-4CD8-A8EC-1DE214EC3A14}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="3015" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{2E473FF1-0CDB-4064-9D38-C9CE84C1A83B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="5" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="Planilha3" sheetId="8" r:id="rId3"/>
     <sheet name="regras" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -136,7 +135,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -483,7 +482,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F64AE8-E54F-41B0-8B93-65E0DA299A73}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -630,11 +629,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFBE0212-22F8-494B-8B0C-84B4FB67E98A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,10 +780,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4336788-DDCE-4FA9-8B66-094EA6C649EE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -819,7 +818,7 @@
       </c>
       <c r="D2" s="2">
         <f ca="1">TODAY()+1</f>
-        <v>44747</v>
+        <v>44769</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -924,11 +923,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A29A6AC-6A66-448B-A573-62859E6CED96}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>